<commit_message>
capturing some testing progress. in general, I'm seeing great agreement between my algorithm and the cspice routine, but my algorithm is a lot more fragile
</commit_message>
<xml_diff>
--- a/testing/testing_spreadsheet.xlsx
+++ b/testing/testing_spreadsheet.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\symmetrical-enigma\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C0CF35-A980-4643-A400-C1C445991167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5475BA4-7AB9-4260-A93A-639F760C6F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D47B664-C2CE-40E7-998A-32DA5E6F4E9F}"/>
+    <workbookView xWindow="-3420" yWindow="4770" windowWidth="7500" windowHeight="6000" xr2:uid="{1D47B664-C2CE-40E7-998A-32DA5E6F4E9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Moon-Sun-Earth" sheetId="1" r:id="rId1"/>
-    <sheet name="Earth-Sun-Moon" sheetId="4" r:id="rId2"/>
-    <sheet name="Titan-Saturn-Earth" sheetId="2" r:id="rId3"/>
-    <sheet name="Saturn-Titan-Earth" sheetId="3" r:id="rId4"/>
+    <sheet name="Titan-Saturn-Earth" sheetId="2" r:id="rId2"/>
+    <sheet name="Saturn-Titan-Earth" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="177">
   <si>
     <t>2030 Jun 01</t>
   </si>
@@ -127,9 +126,6 @@
     <t>TimeAndDate</t>
   </si>
   <si>
-    <t>SymmetricalEnigma</t>
-  </si>
-  <si>
     <t>None.</t>
   </si>
   <si>
@@ -151,9 +147,6 @@
     <t>ANNULAR</t>
   </si>
   <si>
-    <t>Full</t>
-  </si>
-  <si>
     <t>2008 OCT 19 21:29:20.694709</t>
   </si>
   <si>
@@ -440,13 +433,148 @@
   </si>
   <si>
     <t xml:space="preserve">2008 DEC 31 00:59:16.977137 </t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>2008 OCT 19 20:19:55</t>
+  </si>
+  <si>
+    <t>2008 OCT 20 00:01:06</t>
+  </si>
+  <si>
+    <t>2008 NOV 04 19:45:34</t>
+  </si>
+  <si>
+    <t>2008 NOV 05 00:47:05</t>
+  </si>
+  <si>
+    <t>2008 NOV 20 19:17:25</t>
+  </si>
+  <si>
+    <t>2008 NOV 21 00:55:00</t>
+  </si>
+  <si>
+    <t>2008 DEC 06 18:40:02</t>
+  </si>
+  <si>
+    <t>2008 DEC 07 00:32:46</t>
+  </si>
+  <si>
+    <t>2008 DEC 22 17:45:10</t>
+  </si>
+  <si>
+    <t>2008 DEC 22 23:42:25</t>
+  </si>
+  <si>
+    <t>2030 JUN 01 06:20:42</t>
+  </si>
+  <si>
+    <t>2030 JUN 01 06:35:25</t>
+  </si>
+  <si>
+    <t>2030 NOV 25 06:11:50</t>
+  </si>
+  <si>
+    <t>2030 NOV 25 07:29:05</t>
+  </si>
+  <si>
+    <t>2031 MAY 21 06:13:31</t>
+  </si>
+  <si>
+    <t>2031 MAY 21 08:16:21</t>
+  </si>
+  <si>
+    <t>2031 NOV 14 20:17:39</t>
+  </si>
+  <si>
+    <t>2031 NOV 14 21:55:03</t>
+  </si>
+  <si>
+    <t>2034 MAR 20 09:30:15</t>
+  </si>
+  <si>
+    <t>2034 MAR 20 11:04:56</t>
+  </si>
+  <si>
+    <t>2034 SEP 12 15:33:20</t>
+  </si>
+  <si>
+    <t>2034 SEP 12 17:03:19</t>
+  </si>
+  <si>
+    <t>2035 MAR 09 22:27:30</t>
+  </si>
+  <si>
+    <t>2035 MAR 09 23:41:57</t>
+  </si>
+  <si>
+    <t>2035 SEP 02 01:13:32</t>
+  </si>
+  <si>
+    <t>2035 SEP 02 02:37:43</t>
+  </si>
+  <si>
+    <t>2038 JAN 05 13:04:44</t>
+  </si>
+  <si>
+    <t>2038 JAN 05 14:27:22</t>
+  </si>
+  <si>
+    <t>2038 JUL 02 12:29:29</t>
+  </si>
+  <si>
+    <t>2038 JUL 02 14:34:01</t>
+  </si>
+  <si>
+    <t>2038 DEC 26 00:10:36</t>
+  </si>
+  <si>
+    <t>2038 DEC 26 01:47:26</t>
+  </si>
+  <si>
+    <t>SymmetricalEnigma Custom</t>
+  </si>
+  <si>
+    <t>SymmetricalEnigma CSPICE</t>
+  </si>
+  <si>
+    <t>2008 OCT 27 21:35:40</t>
+  </si>
+  <si>
+    <t>2008 OCT 28 01:35:15</t>
+  </si>
+  <si>
+    <t>2008 NOV 12 20:59:59</t>
+  </si>
+  <si>
+    <t>2008 NOV 13 02:25:56</t>
+  </si>
+  <si>
+    <t>2008 NOV 28 20:29:35</t>
+  </si>
+  <si>
+    <t>2008 NOV 29 02:31:16</t>
+  </si>
+  <si>
+    <t>2008 DEC 14 19:46:32</t>
+  </si>
+  <si>
+    <t>2008 DEC 15 02:01:21</t>
+  </si>
+  <si>
+    <t>2008 DEC 30 18:42:28</t>
+  </si>
+  <si>
+    <t>2008 DEC 31 00:59:02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1286,7 +1414,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SymmetricalEnigma</c:v>
+                  <c:v>SymmetricalEnigma CSPICE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2630,13 +2758,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC59B828-E9EE-4E2A-8098-4A4492EAC6D3}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
@@ -2647,10 +2775,11 @@
     <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.7109375" customWidth="1"/>
+    <col min="21" max="21" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2661,11 +2790,14 @@
         <v>28</v>
       </c>
       <c r="P1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="U1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2706,8 +2838,14 @@
         <f>(Q3+R3)/2</f>
         <v>0.2702835648148148</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U3" t="s">
+        <v>143</v>
+      </c>
+      <c r="V3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2748,8 +2886,14 @@
         <f t="shared" ref="S4:S22" si="0">(Q4+R4)/2</f>
         <v>0.2858391203703704</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U4" t="s">
+        <v>145</v>
+      </c>
+      <c r="V4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2790,8 +2934,14 @@
         <f t="shared" si="0"/>
         <v>0.30283564814814812</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U5" t="s">
+        <v>147</v>
+      </c>
+      <c r="V5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2832,8 +2982,14 @@
         <f t="shared" si="0"/>
         <v>0.88020833333333326</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U6" t="s">
+        <v>149</v>
+      </c>
+      <c r="V6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2866,7 +3022,7 @@
       <c r="R7" s="8"/>
       <c r="S7" s="7"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2890,7 +3046,7 @@
       <c r="R8" s="8"/>
       <c r="S8" s="7"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2923,7 +3079,7 @@
       <c r="R9" s="8"/>
       <c r="S9" s="7"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2947,7 +3103,7 @@
       <c r="R10" s="8"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2979,8 +3135,14 @@
         <f t="shared" si="0"/>
         <v>0.42968171296296298</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U11" t="s">
+        <v>151</v>
+      </c>
+      <c r="V11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3021,8 +3183,14 @@
         <f t="shared" si="0"/>
         <v>0.68019097222222225</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U12" t="s">
+        <v>153</v>
+      </c>
+      <c r="V12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3063,8 +3231,14 @@
         <f t="shared" si="0"/>
         <v>0.96241898148148153</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U13" t="s">
+        <v>155</v>
+      </c>
+      <c r="V13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -3105,8 +3279,14 @@
         <f t="shared" si="0"/>
         <v>8.1099537037037039E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U14" t="s">
+        <v>157</v>
+      </c>
+      <c r="V14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -3130,7 +3310,7 @@
       <c r="R15" s="8"/>
       <c r="S15" s="7"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -3163,7 +3343,7 @@
       <c r="R16" s="8"/>
       <c r="S16" s="7"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -3187,7 +3367,7 @@
       <c r="R17" s="8"/>
       <c r="S17" s="7"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -3211,7 +3391,7 @@
       <c r="R18" s="8"/>
       <c r="S18" s="7"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -3235,7 +3415,7 @@
       <c r="R19" s="8"/>
       <c r="S19" s="7"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -3276,8 +3456,14 @@
         <f t="shared" si="0"/>
         <v>0.57444444444444442</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U20" t="s">
+        <v>159</v>
+      </c>
+      <c r="V20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -3318,8 +3504,14 @@
         <f t="shared" si="0"/>
         <v>0.56451388888888887</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U21" t="s">
+        <v>161</v>
+      </c>
+      <c r="V21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3360,8 +3552,14 @@
         <f t="shared" si="0"/>
         <v>4.1782407407407407E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U22" t="s">
+        <v>163</v>
+      </c>
+      <c r="V22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3394,7 +3592,7 @@
       <c r="R23" s="8"/>
       <c r="S23" s="7"/>
     </row>
-    <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" ht="15.75" thickBot="1">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3435,42 +3633,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DF814D-FE06-43AC-BEB3-03E76F7A075E}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E759915E-17EB-43A7-B11D-842AADD44A20}">
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E759915E-17EB-43A7-B11D-842AADD44A20}">
-  <dimension ref="A1:K26"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="0.42578125" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
@@ -3483,494 +3653,527 @@
     <col min="15" max="15" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="14"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="E3" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="14"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="G5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="K5" t="s">
         <v>39</v>
       </c>
-      <c r="J5" t="s">
+    </row>
+    <row r="6" spans="1:14">
+      <c r="F6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="K5" t="s">
+      <c r="G6" s="12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F6" s="12" t="s">
+      <c r="J6" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="K6" t="s">
         <v>43</v>
       </c>
-      <c r="J6" t="s">
+    </row>
+    <row r="7" spans="1:14">
+      <c r="F7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K6" t="s">
+      <c r="G7" s="12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F7" s="12" t="s">
+      <c r="J7" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="K7" t="s">
         <v>47</v>
       </c>
-      <c r="J7" t="s">
+    </row>
+    <row r="8" spans="1:14">
+      <c r="F8" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="K7" t="s">
+      <c r="G8" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F8" s="12" t="s">
+      <c r="J8" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="K8" t="s">
         <v>51</v>
       </c>
-      <c r="J8" t="s">
+    </row>
+    <row r="9" spans="1:14">
+      <c r="F9" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="K8" t="s">
+      <c r="G9" s="12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F9" s="12" t="s">
+      <c r="J9" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="K9" t="s">
         <v>55</v>
       </c>
-      <c r="J9" t="s">
+    </row>
+    <row r="11" spans="1:14">
+      <c r="B11" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="K9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
-        <v>58</v>
-      </c>
       <c r="C11" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" t="str">
-        <f>TRIM(B11)</f>
+        <f t="shared" ref="F11:F26" si="0">TRIM(B11)</f>
         <v>2008 OCT 19 20:44:30.377189</v>
       </c>
       <c r="G11" t="str">
-        <f>TRIM(C11)</f>
+        <f t="shared" ref="G11:G26" si="1">TRIM(C11)</f>
         <v>2008 OCT 19 21:29:20.694709</v>
       </c>
       <c r="J11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="B12" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="K11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>61</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" t="str">
-        <f>TRIM(B12)</f>
+        <f t="shared" si="0"/>
         <v>2008 OCT 19 22:53:34.442728</v>
       </c>
       <c r="G12" t="str">
-        <f>TRIM(C12)</f>
+        <f t="shared" si="1"/>
         <v>2008 OCT 19 23:38:26.219865</v>
       </c>
       <c r="J12" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="B13" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="K12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>64</v>
-      </c>
       <c r="C13" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" t="str">
-        <f>TRIM(B13)</f>
+        <f t="shared" si="0"/>
         <v>2008 NOV 04 19:54:40.368045</v>
       </c>
       <c r="G13" t="str">
-        <f>TRIM(C13)</f>
+        <f t="shared" si="1"/>
         <v>2008 NOV 04 20:15:38.652650</v>
       </c>
       <c r="J13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="B14" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>65</v>
-      </c>
-      <c r="K13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>67</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" t="str">
-        <f>TRIM(B14)</f>
+        <f t="shared" si="0"/>
         <v>2008 NOV 05 00:18:59.130645</v>
       </c>
       <c r="G14" t="str">
-        <f>TRIM(C14)</f>
+        <f t="shared" si="1"/>
         <v>2008 NOV 05 00:39:58.607159</v>
       </c>
       <c r="J14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="B15" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="K14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
-        <v>70</v>
-      </c>
       <c r="C15" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" t="str">
-        <f>TRIM(B15)</f>
+        <f t="shared" si="0"/>
         <v>2008 NOV 20 19:21:46.714396</v>
       </c>
       <c r="G15" t="str">
-        <f>TRIM(C15)</f>
+        <f t="shared" si="1"/>
         <v>2008 NOV 20 19:38:59.674043</v>
       </c>
       <c r="J15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="K15" t="s">
+      <c r="C16" s="13" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>74</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" t="str">
-        <f>TRIM(B16)</f>
+        <f t="shared" si="0"/>
         <v>2008 NOV 21 00:35:26.726756</v>
       </c>
       <c r="G16" t="str">
-        <f>TRIM(C16)</f>
+        <f t="shared" si="1"/>
         <v>2008 NOV 21 00:52:40.606954</v>
       </c>
       <c r="J16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="B17" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="K16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
-        <v>77</v>
-      </c>
       <c r="C17" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" t="str">
-        <f>TRIM(B17)</f>
+        <f t="shared" si="0"/>
         <v>2008 DEC 06 18:42:36.120122</v>
       </c>
       <c r="G17" t="str">
-        <f>TRIM(C17)</f>
+        <f t="shared" si="1"/>
         <v>2008 DEC 06 18:58:34.093679</v>
       </c>
       <c r="J17" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="B18" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="K17" t="s">
+      <c r="C18" s="13" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" t="str">
-        <f>TRIM(B18)</f>
+        <f t="shared" si="0"/>
         <v>2008 DEC 07 00:16:17.653066</v>
       </c>
       <c r="G18" t="str">
-        <f>TRIM(C18)</f>
+        <f t="shared" si="1"/>
         <v>2008 DEC 07 00:32:16.331199</v>
       </c>
       <c r="J18" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="B19" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="K18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
-        <v>84</v>
-      </c>
       <c r="C19" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" t="str">
-        <f>TRIM(B19)</f>
+        <f t="shared" si="0"/>
         <v>2008 DEC 22 17:47:10.796147</v>
       </c>
       <c r="G19" t="str">
-        <f>TRIM(C19)</f>
+        <f t="shared" si="1"/>
         <v>2008 DEC 22 18:02:46.308375</v>
       </c>
       <c r="J19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="B20" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="K19" t="s">
+      <c r="C20" s="13" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>88</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" t="str">
-        <f>TRIM(B20)</f>
+        <f t="shared" si="0"/>
         <v>2008 DEC 22 23:26:52.721881</v>
       </c>
       <c r="G20" t="str">
-        <f>TRIM(C20)</f>
+        <f t="shared" si="1"/>
         <v>2008 DEC 22 23:42:28.860689</v>
       </c>
       <c r="J20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" t="str">
-        <f>TRIM(B21)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G21" t="str">
-        <f>TRIM(C21)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="B22" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F22" t="str">
-        <f>TRIM(B22)</f>
+        <f t="shared" si="0"/>
         <v>2008 OCT 19 20:44:30.377189</v>
       </c>
       <c r="G22" t="str">
-        <f>TRIM(C22)</f>
+        <f t="shared" si="1"/>
         <v>2008 OCT 19 23:38:26.219865</v>
       </c>
       <c r="J22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="N22" t="s">
+        <v>133</v>
+      </c>
+      <c r="O22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="B23" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
       <c r="F23" t="str">
-        <f>TRIM(B23)</f>
+        <f t="shared" si="0"/>
         <v>2008 NOV 04 19:54:40.368045</v>
       </c>
       <c r="G23" t="str">
-        <f>TRIM(C23)</f>
+        <f t="shared" si="1"/>
         <v>2008 NOV 05 00:39:58.607159</v>
       </c>
       <c r="J23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="N23" t="s">
+        <v>135</v>
+      </c>
+      <c r="O23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="B24" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" t="str">
-        <f>TRIM(B24)</f>
+        <f t="shared" si="0"/>
         <v>2008 NOV 20 19:21:46.714396</v>
       </c>
       <c r="G24" t="str">
-        <f>TRIM(C24)</f>
+        <f t="shared" si="1"/>
         <v>2008 NOV 21 00:52:40.606954</v>
       </c>
       <c r="J24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="N24" t="s">
+        <v>137</v>
+      </c>
+      <c r="O24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="B25" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
       <c r="F25" t="str">
-        <f>TRIM(B25)</f>
+        <f t="shared" si="0"/>
         <v>2008 DEC 06 18:42:36.120122</v>
       </c>
       <c r="G25" t="str">
-        <f>TRIM(C25)</f>
+        <f t="shared" si="1"/>
         <v>2008 DEC 07 00:32:16.331199</v>
       </c>
       <c r="J25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="N25" t="s">
+        <v>139</v>
+      </c>
+      <c r="O25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="B26" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" t="str">
-        <f>TRIM(B26)</f>
+        <f t="shared" si="0"/>
         <v>2008 DEC 22 17:47:10.796147</v>
       </c>
       <c r="G26" t="str">
-        <f>TRIM(C26)</f>
+        <f t="shared" si="1"/>
         <v>2008 DEC 22 23:42:28.860689</v>
       </c>
       <c r="J26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K26" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="N26" t="s">
+        <v>141</v>
+      </c>
+      <c r="O26" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3979,326 +4182,360 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C57BFE7-26EC-4C5C-BB8E-1929B2489846}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="B5" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="B6" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B10" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="12" t="s">
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" t="s">
         <v>95</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F12" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="C13" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" t="s">
         <v>99</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" s="12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="C15" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" t="s">
         <v>103</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F16" t="s">
+        <v>125</v>
+      </c>
+      <c r="G16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="B17" s="12" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="C17" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" t="s">
         <v>107</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="B18" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F18" t="s">
+        <v>129</v>
+      </c>
+      <c r="G18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="B19" s="12" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="C19" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" t="s">
         <v>111</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="G6" t="s">
+      <c r="C21" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="G21" t="s">
         <v>115</v>
       </c>
-      <c r="G10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" s="12" t="s">
+      <c r="J21" t="s">
+        <v>167</v>
+      </c>
+      <c r="K21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="B22" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="F11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="C22" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G22" t="s">
         <v>119</v>
       </c>
-      <c r="G12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="12" t="s">
+      <c r="J22" t="s">
+        <v>169</v>
+      </c>
+      <c r="K22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="B23" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="F13" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="C23" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G23" t="s">
         <v>123</v>
       </c>
-      <c r="G14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="12" t="s">
+      <c r="J23" t="s">
+        <v>171</v>
+      </c>
+      <c r="K23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="B24" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="C24" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G24" t="s">
         <v>127</v>
       </c>
-      <c r="G16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="12" t="s">
+      <c r="J24" t="s">
+        <v>173</v>
+      </c>
+      <c r="K24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="B25" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="F17" t="s">
-        <v>109</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="C25" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="G25" t="s">
         <v>131</v>
       </c>
-      <c r="G18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="F19" t="s">
-        <v>113</v>
-      </c>
-      <c r="G19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F21" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F22" t="s">
-        <v>119</v>
-      </c>
-      <c r="G22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="F23" t="s">
-        <v>123</v>
-      </c>
-      <c r="G23" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="F24" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="F25" t="s">
-        <v>131</v>
-      </c>
-      <c r="G25" t="s">
-        <v>133</v>
+      <c r="J25" t="s">
+        <v>175</v>
+      </c>
+      <c r="K25" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>